<commit_message>
[CAN-15] TXPL testcase testbench
</commit_message>
<xml_diff>
--- a/CAN_merge/Test Cases/tx_priority_testcases.xlsx
+++ b/CAN_merge/Test Cases/tx_priority_testcases.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23001"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\djste\Documents\GitHub\CAN_we_do_it_Can_Controller\Documentations\Test Cases\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\40010371\Documents\Can Controller\Test Cases\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F973FE9D-7421-4ED4-817D-A6114418613F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{7B8C92B5-316F-47D4-98E1-A91E1B0DF0FA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11010" yWindow="0" windowWidth="15795" windowHeight="11385" xr2:uid="{6D9DD170-8ED8-4417-B493-FE566D307589}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{6D9DD170-8ED8-4417-B493-FE566D307589}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="102">
   <si>
     <t>Requirement Tag</t>
   </si>
@@ -379,12 +379,18 @@
 'i_tx_empty'  = 0
 'i_hpbfull' = 0</t>
   </si>
+  <si>
+    <t>PASS</t>
+  </si>
+  <si>
+    <t>7fe72fd</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -419,13 +425,34 @@
       <family val="1"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -437,12 +464,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -470,14 +497,27 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -792,412 +832,585 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{73642E39-ECFF-4314-AFC1-488407319D91}">
   <dimension ref="A1:I22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B9" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="K6" sqref="K6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="33.28515625" customWidth="1"/>
-    <col min="2" max="2" width="22" customWidth="1"/>
-    <col min="3" max="3" width="47.5703125" customWidth="1"/>
-    <col min="4" max="4" width="62.42578125" customWidth="1"/>
-    <col min="5" max="5" width="31" customWidth="1"/>
-    <col min="6" max="6" width="47.140625" customWidth="1"/>
-    <col min="7" max="7" width="34.85546875" customWidth="1"/>
-    <col min="8" max="8" width="14.28515625" customWidth="1"/>
-    <col min="9" max="9" width="15.42578125" customWidth="1"/>
+    <col min="1" max="1" width="16.109375" style="9" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.33203125" style="6" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="47.5546875" customWidth="1"/>
+    <col min="4" max="4" width="54.109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="38.88671875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.33203125" customWidth="1"/>
+    <col min="9" max="9" width="15.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="I1" s="11" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="80.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    <row r="2" spans="1:9" ht="80.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="C2" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="D2" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="E2" s="9" t="s">
+      <c r="E2" s="8" t="s">
         <v>53</v>
       </c>
-      <c r="F2" s="8" t="s">
+      <c r="F2" s="7" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="3" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="G2" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="H2" s="10" t="s">
+        <v>100</v>
+      </c>
+      <c r="I2" s="12" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A3" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C3" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="D3" s="10" t="s">
+      <c r="D3" s="14" t="s">
         <v>65</v>
       </c>
-      <c r="E3" s="7"/>
-      <c r="F3" s="10" t="s">
+      <c r="E3" s="6"/>
+      <c r="F3" s="14" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="H3" s="10" t="s">
+        <v>100</v>
+      </c>
+      <c r="I3" s="12" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A4" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="C4" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="D4" s="10"/>
-      <c r="E4" s="7"/>
-      <c r="F4" s="10"/>
-    </row>
-    <row r="5" spans="1:9" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+      <c r="D4" s="14"/>
+      <c r="E4" s="6"/>
+      <c r="F4" s="14"/>
+      <c r="H4" s="10" t="s">
+        <v>100</v>
+      </c>
+      <c r="I4" s="12" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="30.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="C5" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="D5" s="10"/>
-      <c r="E5" s="7"/>
-      <c r="F5" s="10"/>
-    </row>
-    <row r="6" spans="1:9" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+      <c r="D5" s="14"/>
+      <c r="E5" s="6"/>
+      <c r="F5" s="14"/>
+      <c r="H5" s="10" t="s">
+        <v>100</v>
+      </c>
+      <c r="I5" s="12" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="45" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="C6" s="2" t="s">
+      <c r="C6" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="D6" s="10"/>
-      <c r="E6" s="7"/>
-      <c r="F6" s="10"/>
-    </row>
-    <row r="7" spans="1:9" ht="68.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+      <c r="D6" s="14"/>
+      <c r="E6" s="6"/>
+      <c r="F6" s="14"/>
+      <c r="H6" s="10" t="s">
+        <v>100</v>
+      </c>
+      <c r="I6" s="12" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="68.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="C7" s="2" t="s">
+      <c r="C7" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="D7" s="10"/>
-      <c r="E7" s="7"/>
-      <c r="F7" s="10"/>
-    </row>
-    <row r="8" spans="1:9" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+      <c r="D7" s="14"/>
+      <c r="E7" s="6"/>
+      <c r="F7" s="14"/>
+      <c r="H7" s="10" t="s">
+        <v>100</v>
+      </c>
+      <c r="I7" s="12" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="45" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="C8" s="2" t="s">
+      <c r="C8" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="D8" s="11" t="s">
+      <c r="D8" s="15" t="s">
         <v>66</v>
       </c>
-      <c r="E8" s="7"/>
-      <c r="F8" s="9" t="s">
+      <c r="E8" s="6"/>
+      <c r="F8" s="8" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="9" spans="1:9" ht="69" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+      <c r="G8" s="8" t="s">
+        <v>86</v>
+      </c>
+      <c r="H8" s="10" t="s">
+        <v>100</v>
+      </c>
+      <c r="I8" s="12" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" ht="69" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="C9" s="2" t="s">
+      <c r="C9" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="D9" s="11"/>
-      <c r="E9" s="9" t="s">
+      <c r="D9" s="15"/>
+      <c r="E9" s="8" t="s">
         <v>53</v>
       </c>
-      <c r="F9" s="9" t="s">
+      <c r="F9" s="8" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="10" spans="1:9" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+      <c r="G9" s="8" t="s">
+        <v>86</v>
+      </c>
+      <c r="H9" s="10" t="s">
+        <v>100</v>
+      </c>
+      <c r="I9" s="12" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" ht="50.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="C10" s="2" t="s">
+      <c r="C10" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="D10" s="11"/>
-      <c r="E10" s="7"/>
-      <c r="F10" s="9" t="s">
+      <c r="D10" s="15"/>
+      <c r="E10" s="6"/>
+      <c r="F10" s="8" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="11" spans="1:9" ht="75.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+      <c r="G10" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="H10" s="10" t="s">
+        <v>100</v>
+      </c>
+      <c r="I10" s="12" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" ht="75.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B11" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="C11" s="2" t="s">
+      <c r="C11" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="D11" s="6" t="s">
+      <c r="D11" s="5" t="s">
         <v>97</v>
       </c>
-      <c r="E11" s="8" t="s">
+      <c r="E11" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="F11" s="9" t="s">
+      <c r="F11" s="8" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="12" spans="1:9" ht="59.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
+      <c r="G11" s="8" t="s">
+        <v>87</v>
+      </c>
+      <c r="H11" s="10" t="s">
+        <v>100</v>
+      </c>
+      <c r="I11" s="12" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" ht="59.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B12" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="C12" s="2" t="s">
+      <c r="C12" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="D12" s="4" t="s">
+      <c r="D12" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="E12" s="8" t="s">
+      <c r="E12" s="7" t="s">
         <v>98</v>
       </c>
-      <c r="F12" s="9" t="s">
+      <c r="F12" s="8" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="13" spans="1:9" ht="57" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
+      <c r="G12" s="8" t="s">
+        <v>88</v>
+      </c>
+      <c r="H12" s="10" t="s">
+        <v>100</v>
+      </c>
+      <c r="I12" s="12" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" ht="57" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B13" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="C13" s="2" t="s">
+      <c r="C13" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="D13" s="12" t="s">
+      <c r="D13" s="13" t="s">
         <v>59</v>
       </c>
-      <c r="E13" s="7"/>
-      <c r="F13" s="9" t="s">
+      <c r="E13" s="6"/>
+      <c r="F13" s="8" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="14" spans="1:9" ht="71.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
+      <c r="G13" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="H13" s="10" t="s">
+        <v>100</v>
+      </c>
+      <c r="I13" s="12" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" ht="71.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B14" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="C14" s="2" t="s">
+      <c r="C14" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="D14" s="12"/>
-      <c r="E14" s="7"/>
-      <c r="F14" s="9" t="s">
+      <c r="D14" s="13"/>
+      <c r="E14" s="6"/>
+      <c r="F14" s="8" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="15" spans="1:9" ht="55.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
+      <c r="G14" s="8" t="s">
+        <v>89</v>
+      </c>
+      <c r="H14" s="10" t="s">
+        <v>100</v>
+      </c>
+      <c r="I14" s="12" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" ht="55.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B15" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="C15" s="2" t="s">
+      <c r="C15" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="D15" s="2" t="s">
+      <c r="D15" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="E15" s="7"/>
-      <c r="F15" s="9" t="s">
+      <c r="E15" s="6"/>
+      <c r="F15" s="8" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="16" spans="1:9" ht="96" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
+      <c r="G15" s="8" t="s">
+        <v>90</v>
+      </c>
+      <c r="H15" s="10" t="s">
+        <v>100</v>
+      </c>
+      <c r="I15" s="12" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" ht="96" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B16" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="C16" s="2" t="s">
+      <c r="C16" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="D16" s="4" t="s">
+      <c r="D16" s="3" t="s">
         <v>96</v>
       </c>
-      <c r="E16" s="8" t="s">
+      <c r="E16" s="7" t="s">
         <v>99</v>
       </c>
-      <c r="F16" s="9" t="s">
+      <c r="F16" s="8" t="s">
         <v>91</v>
       </c>
-    </row>
-    <row r="17" spans="1:6" ht="61.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
+      <c r="G16" s="8" t="s">
+        <v>91</v>
+      </c>
+      <c r="H16" s="10" t="s">
+        <v>100</v>
+      </c>
+      <c r="I16" s="12" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" ht="61.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B17" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="C17" s="5" t="s">
+      <c r="C17" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="D17" s="12" t="s">
+      <c r="D17" s="13" t="s">
         <v>61</v>
       </c>
-      <c r="E17" s="7"/>
-      <c r="F17" s="9" t="s">
+      <c r="E17" s="6"/>
+      <c r="F17" s="8" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="18" spans="1:6" ht="56.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
+      <c r="G17" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="H17" s="10" t="s">
+        <v>100</v>
+      </c>
+      <c r="I17" s="12" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" ht="56.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B18" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="C18" s="2" t="s">
+      <c r="C18" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="D18" s="12"/>
-      <c r="E18" s="7"/>
-      <c r="F18" s="9" t="s">
+      <c r="D18" s="13"/>
+      <c r="E18" s="6"/>
+      <c r="F18" s="8" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="19" spans="1:6" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
+      <c r="G18" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="H18" s="10" t="s">
+        <v>100</v>
+      </c>
+      <c r="I18" s="12" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" ht="46.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B19" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="C19" s="2" t="s">
+      <c r="C19" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="D19" s="12" t="s">
+      <c r="D19" s="13" t="s">
         <v>92</v>
       </c>
-      <c r="E19" s="7"/>
-      <c r="F19" s="9" t="s">
+      <c r="E19" s="6"/>
+      <c r="F19" s="8" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="20" spans="1:6" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
+      <c r="G19" s="8" t="s">
+        <v>90</v>
+      </c>
+      <c r="H19" s="10" t="s">
+        <v>100</v>
+      </c>
+      <c r="I19" s="12" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" ht="45.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="B20" t="s">
+      <c r="B20" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="C20" s="2" t="s">
+      <c r="C20" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="D20" s="12"/>
-      <c r="E20" s="7"/>
-      <c r="F20" s="9" t="s">
+      <c r="D20" s="13"/>
+      <c r="E20" s="6"/>
+      <c r="F20" s="8" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="21" spans="1:6" ht="48" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
+      <c r="G20" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="H20" s="10" t="s">
+        <v>100</v>
+      </c>
+      <c r="I20" s="12" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" ht="48" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="9" t="s">
         <v>67</v>
       </c>
-      <c r="B21" t="s">
+      <c r="B21" s="6" t="s">
         <v>83</v>
       </c>
-      <c r="C21" s="3" t="s">
+      <c r="C21" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="D21" s="12"/>
-      <c r="E21" s="7"/>
-      <c r="F21" s="9" t="s">
+      <c r="D21" s="13"/>
+      <c r="E21" s="6"/>
+      <c r="F21" s="8" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="22" spans="1:6" ht="57" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
+      <c r="G21" s="8" t="s">
+        <v>93</v>
+      </c>
+      <c r="H21" s="10" t="s">
+        <v>100</v>
+      </c>
+      <c r="I21" s="12" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" ht="57" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="9" t="s">
         <v>85</v>
       </c>
-      <c r="B22" t="s">
+      <c r="B22" s="6" t="s">
         <v>84</v>
       </c>
-      <c r="C22" s="2" t="s">
+      <c r="C22" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="D22" s="2" t="s">
+      <c r="D22" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="E22" s="8" t="s">
+      <c r="E22" s="7" t="s">
         <v>95</v>
       </c>
-      <c r="F22" s="9" t="s">
+      <c r="F22" s="8" t="s">
         <v>87</v>
+      </c>
+      <c r="G22" s="8" t="s">
+        <v>87</v>
+      </c>
+      <c r="H22" s="10" t="s">
+        <v>100</v>
+      </c>
+      <c r="I22" s="12" t="s">
+        <v>101</v>
       </c>
     </row>
   </sheetData>
@@ -1210,7 +1423,30 @@
     <mergeCell ref="D17:D18"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
+  <hyperlinks>
+    <hyperlink ref="I2" r:id="rId1" display="https://github.com/Nemiland/CAN-Controller/commit/7fe72fdc46e82eb0b1fb8341e83c9e45a4b06a31" xr:uid="{C1D2C68E-5BE4-494D-9F0B-414FCE950521}"/>
+    <hyperlink ref="I3" r:id="rId2" display="https://github.com/Nemiland/CAN-Controller/commit/7fe72fdc46e82eb0b1fb8341e83c9e45a4b06a31" xr:uid="{9D45CB9D-3C2E-4136-B57E-F594D99DB22F}"/>
+    <hyperlink ref="I4" r:id="rId3" display="https://github.com/Nemiland/CAN-Controller/commit/7fe72fdc46e82eb0b1fb8341e83c9e45a4b06a31" xr:uid="{C930A397-733A-4EAC-BD06-B28DC99D00B9}"/>
+    <hyperlink ref="I5" r:id="rId4" display="https://github.com/Nemiland/CAN-Controller/commit/7fe72fdc46e82eb0b1fb8341e83c9e45a4b06a31" xr:uid="{859F8CAD-0CDB-4DDD-A5D5-8F989AD99C42}"/>
+    <hyperlink ref="I6" r:id="rId5" display="https://github.com/Nemiland/CAN-Controller/commit/7fe72fdc46e82eb0b1fb8341e83c9e45a4b06a31" xr:uid="{A3471B8C-0CF6-4766-9405-F7171F8C37B8}"/>
+    <hyperlink ref="I7" r:id="rId6" display="https://github.com/Nemiland/CAN-Controller/commit/7fe72fdc46e82eb0b1fb8341e83c9e45a4b06a31" xr:uid="{0CCA7731-DCA1-4458-B919-4F3DFE71C732}"/>
+    <hyperlink ref="I8" r:id="rId7" display="https://github.com/Nemiland/CAN-Controller/commit/7fe72fdc46e82eb0b1fb8341e83c9e45a4b06a31" xr:uid="{37DE2BEC-56A6-4399-AD8E-FE369690CB67}"/>
+    <hyperlink ref="I9" r:id="rId8" display="https://github.com/Nemiland/CAN-Controller/commit/7fe72fdc46e82eb0b1fb8341e83c9e45a4b06a31" xr:uid="{04C4E435-4038-4D68-921E-6AFCE1DD6385}"/>
+    <hyperlink ref="I10" r:id="rId9" display="https://github.com/Nemiland/CAN-Controller/commit/7fe72fdc46e82eb0b1fb8341e83c9e45a4b06a31" xr:uid="{10BD90A3-DA3E-4F8A-ABC2-5FB40CF50F71}"/>
+    <hyperlink ref="I11" r:id="rId10" display="https://github.com/Nemiland/CAN-Controller/commit/7fe72fdc46e82eb0b1fb8341e83c9e45a4b06a31" xr:uid="{C6B35B5D-0836-48B0-871A-1D8626B41F06}"/>
+    <hyperlink ref="I12" r:id="rId11" display="https://github.com/Nemiland/CAN-Controller/commit/7fe72fdc46e82eb0b1fb8341e83c9e45a4b06a31" xr:uid="{64F15B18-35BC-4B18-9145-F45613368F04}"/>
+    <hyperlink ref="I13" r:id="rId12" display="https://github.com/Nemiland/CAN-Controller/commit/7fe72fdc46e82eb0b1fb8341e83c9e45a4b06a31" xr:uid="{CCC97F09-AB48-4DFE-9512-8F69A568BC8F}"/>
+    <hyperlink ref="I14" r:id="rId13" display="https://github.com/Nemiland/CAN-Controller/commit/7fe72fdc46e82eb0b1fb8341e83c9e45a4b06a31" xr:uid="{4EB90709-FF79-459D-85B6-780A228B6B19}"/>
+    <hyperlink ref="I15" r:id="rId14" display="https://github.com/Nemiland/CAN-Controller/commit/7fe72fdc46e82eb0b1fb8341e83c9e45a4b06a31" xr:uid="{5F04363F-5C21-450D-8BB8-7393DEBAFC0D}"/>
+    <hyperlink ref="I16" r:id="rId15" display="https://github.com/Nemiland/CAN-Controller/commit/7fe72fdc46e82eb0b1fb8341e83c9e45a4b06a31" xr:uid="{8734FAF3-23EB-4229-8C78-9D9FF28C11FC}"/>
+    <hyperlink ref="I17" r:id="rId16" display="https://github.com/Nemiland/CAN-Controller/commit/7fe72fdc46e82eb0b1fb8341e83c9e45a4b06a31" xr:uid="{3C204232-0DAD-4A47-9568-0C0328FF051B}"/>
+    <hyperlink ref="I18" r:id="rId17" display="https://github.com/Nemiland/CAN-Controller/commit/7fe72fdc46e82eb0b1fb8341e83c9e45a4b06a31" xr:uid="{F9C77FF3-42F3-4A2F-84B1-3B17D6566EF0}"/>
+    <hyperlink ref="I19" r:id="rId18" display="https://github.com/Nemiland/CAN-Controller/commit/7fe72fdc46e82eb0b1fb8341e83c9e45a4b06a31" xr:uid="{6FE791ED-C87F-43A0-8D44-3051EF9B25E9}"/>
+    <hyperlink ref="I20" r:id="rId19" display="https://github.com/Nemiland/CAN-Controller/commit/7fe72fdc46e82eb0b1fb8341e83c9e45a4b06a31" xr:uid="{7A673871-0D0D-4B2E-AE88-098B297613C5}"/>
+    <hyperlink ref="I21" r:id="rId20" display="https://github.com/Nemiland/CAN-Controller/commit/7fe72fdc46e82eb0b1fb8341e83c9e45a4b06a31" xr:uid="{84AF4E4E-FE00-4F9B-966E-2F54118BD01D}"/>
+    <hyperlink ref="I22" r:id="rId21" display="https://github.com/Nemiland/CAN-Controller/commit/7fe72fdc46e82eb0b1fb8341e83c9e45a4b06a31" xr:uid="{DCAF5ED8-BD28-43A9-83A5-C432D28608DB}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId22"/>
 </worksheet>
 </file>
</xml_diff>